<commit_message>
Add updated fish temperature  suitability from Dibble new report
Also reorganized Bryce's data into subfolder
Added more river temperature data
</commit_message>
<xml_diff>
--- a/LakePowellTemperatureScenarios/FishTemperatureRequirements.xlsx
+++ b/LakePowellTemperatureScenarios/FishTemperatureRequirements.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20363"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20368"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverFutures\LakePowellTemperatureScenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6534BF5C-E3A0-4DC7-BDE0-AA502520F768}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31044408-EF4E-4D0A-BCFF-7E253B2C7915}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7950" activeTab="1" xr2:uid="{4163B5F8-470B-4BB8-AE08-86093EE151C8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7950" activeTab="3" xr2:uid="{4163B5F8-470B-4BB8-AE08-86093EE151C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="3" r:id="rId1"/>
     <sheet name="TempRequirements" sheetId="1" r:id="rId2"/>
     <sheet name="MinTDD" sheetId="2" r:id="rId3"/>
+    <sheet name="TempDibble" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="121">
   <si>
     <t>Common Name</t>
   </si>
@@ -333,6 +334,68 @@
   </si>
   <si>
     <t>Keystone</t>
+  </si>
+  <si>
+    <t>Maximum</t>
+  </si>
+  <si>
+    <t>Minimum</t>
+  </si>
+  <si>
+    <t>Minimum Optimal</t>
+  </si>
+  <si>
+    <t>Maximum Optimal</t>
+  </si>
+  <si>
+    <t>Colorado Pikeminnow</t>
+  </si>
+  <si>
+    <t>References</t>
+  </si>
+  <si>
+    <t>Bulkley et al. 1981, Black and Bulkley 1985, Osmundson 1987, Petersen and Paukert 2005, Bestgenet al. 2006, Lamarra 2007,Osmundson 2011, Valdez et al. 2013)Razorback Sucker 14 21 31 37 (Bulkley and Pimentel 1983, Carvethet al. 2006, Lamarra 2007, Bestgen2008, Valdez et al. 2013, USFWS2018)</t>
+  </si>
+  <si>
+    <t>Humpback Chub</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (Hamman 1982, Gorman andVanHoosen 2000, Voichick andWright 2007 [pre-dam watertemperatures], Dzul et al. 2017,USFWS 2017, Yackulic et al. 2018,USGS WaterWatch Data: Station09383100)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Smallmouth Bass  </t>
+  </si>
+  <si>
+    <t>(CobleJobling 1981, Smale and Rabeni1995, Bestgen and Hill 2016b)Red Shiner 16 22 30 38 (Gale 1986, Smale and Rabeni 1995,Lentsch et al. 1996, Carveth et al.2006, Peterson 2017)</t>
+  </si>
+  <si>
+    <t>Channel Catfish</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (Shrable et al. 1969, Andrews andStickney 1972, Cheetham et al. 1976,Jobling 1981, McMahon and Terrell1982, Wellborn 1990, Buentello et al.2000, Lamarra 2007, Valdez et al. 2013</t>
+  </si>
+  <si>
+    <t>Razorback Sucker</t>
+  </si>
+  <si>
+    <t>(Bulkley and Pimentel 1983, Carveth
+et al. 2006, Lamarra 2007, Bestgen
+2008, Valdez et al. 2013, USFWS
+2018)</t>
+  </si>
+  <si>
+    <t>Red Shiner</t>
+  </si>
+  <si>
+    <t>Gale 1986, Smale and Rabeni 1995,
+Lentsch et al. 1996, Carveth et al.
+2006, Peterson 2017)</t>
+  </si>
+  <si>
+    <t>TempDibble</t>
+  </si>
+  <si>
+    <t>Updated requirements from Dibble et al (2020, submitted), Table S1, page 39</t>
   </si>
 </sst>
 </file>
@@ -368,12 +431,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -688,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A29FBA0E-4F01-4E3C-99AE-8101B3600499}">
-  <dimension ref="C1:D7"/>
+  <dimension ref="C1:D8"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -739,6 +803,14 @@
         <v>97</v>
       </c>
     </row>
+    <row r="8" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C8" t="s">
+        <v>119</v>
+      </c>
+      <c r="D8" t="s">
+        <v>120</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -748,8 +820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EC18E6D-F6CE-4B94-B35B-DF1457A60E0C}">
   <dimension ref="A1:N36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3528,4 +3600,206 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93320355-63E3-4857-AA4B-7C74619B5FDE}">
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.26953125" customWidth="1"/>
+    <col min="2" max="2" width="6.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2">
+        <v>13</v>
+      </c>
+      <c r="E2">
+        <v>22</v>
+      </c>
+      <c r="F2">
+        <v>31</v>
+      </c>
+      <c r="G2">
+        <v>37</v>
+      </c>
+      <c r="H2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3">
+        <v>14</v>
+      </c>
+      <c r="E3">
+        <v>21</v>
+      </c>
+      <c r="F3">
+        <v>31</v>
+      </c>
+      <c r="G3">
+        <v>37</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4">
+        <v>12</v>
+      </c>
+      <c r="E4">
+        <v>16</v>
+      </c>
+      <c r="F4">
+        <v>30</v>
+      </c>
+      <c r="G4">
+        <v>37</v>
+      </c>
+      <c r="H4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D5">
+        <v>16</v>
+      </c>
+      <c r="E5">
+        <v>25</v>
+      </c>
+      <c r="F5">
+        <v>29</v>
+      </c>
+      <c r="G5">
+        <v>37</v>
+      </c>
+      <c r="H5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D6">
+        <v>16</v>
+      </c>
+      <c r="E6">
+        <v>22</v>
+      </c>
+      <c r="F6">
+        <v>30</v>
+      </c>
+      <c r="G6">
+        <v>38</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D7">
+        <v>18</v>
+      </c>
+      <c r="E7">
+        <v>26</v>
+      </c>
+      <c r="F7">
+        <v>30</v>
+      </c>
+      <c r="G7">
+        <v>35</v>
+      </c>
+      <c r="H7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>